<commit_message>
fixed stationID not unique key bug
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Rothfels\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Rothfels\Documents\auto_qc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B3AD79-7CF6-4C0C-BF22-7A01728E644A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38CE5C6-1CE6-452B-81C2-D15958595509}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8175" xr2:uid="{DA3D1637-7497-4FA4-AFD8-B0930C0FCFB0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8175" activeTab="2" xr2:uid="{DA3D1637-7497-4FA4-AFD8-B0930C0FCFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>File</t>
   </si>
@@ -200,7 +200,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,6 +229,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -297,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,6 +329,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -721,9 +730,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{328796CE-C1EE-4EC0-BFDD-AD4395456B69}">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +778,7 @@
       <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -778,7 +787,7 @@
       <c r="N1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="10" t="s">
         <v>10</v>
       </c>
       <c r="P1" s="4" t="s">
@@ -787,7 +796,7 @@
       <c r="Q1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="10" t="s">
         <v>13</v>
       </c>
       <c r="S1" s="4" t="s">
@@ -847,102 +856,105 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661158B2-352C-4F57-9B9E-C73E8105ACCC}">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N23" sqref="N23"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="24" max="24" width="20.5703125" customWidth="1"/>
-    <col min="25" max="25" width="11.140625" style="8" customWidth="1"/>
-    <col min="26" max="26" width="11.85546875" customWidth="1"/>
+    <col min="25" max="25" width="20.5703125" customWidth="1"/>
+    <col min="26" max="26" width="11.140625" style="8" customWidth="1"/>
+    <col min="27" max="27" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Z1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="AA1" s="9" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="Z2:Z104857 Y2:Y104857">
+  <conditionalFormatting sqref="Z2:AA104857">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"O"</formula>
     </cfRule>

</xml_diff>

<commit_message>
added mdb file name to drops list
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Rothfels\Documents\auto_qc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38CE5C6-1CE6-452B-81C2-D15958595509}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D986C827-F299-429F-BBA5-308F7A6B7D21}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8175" activeTab="2" xr2:uid="{DA3D1637-7497-4FA4-AFD8-B0930C0FCFB0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8175" xr2:uid="{DA3D1637-7497-4FA4-AFD8-B0930C0FCFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>File</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>GPS Check</t>
-  </si>
-  <si>
-    <t>Decreasing Deflection</t>
   </si>
   <si>
     <t>Comments</t>
@@ -153,9 +150,6 @@
 </t>
   </si>
   <si>
-    <t>Increasing Deflections</t>
-  </si>
-  <si>
     <t>insufficient field tests</t>
   </si>
   <si>
@@ -166,6 +160,9 @@
   </si>
   <si>
     <t>Insufficient Field Tests</t>
+  </si>
+  <si>
+    <t>Decreasing Deflections</t>
   </si>
 </sst>
 </file>
@@ -730,9 +727,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{328796CE-C1EE-4EC0-BFDD-AD4395456B69}">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,13 +743,13 @@
   <sheetData>
     <row r="1" spans="1:21" ht="54" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>0</v>
@@ -773,7 +770,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>6</v>
@@ -800,13 +797,13 @@
         <v>13</v>
       </c>
       <c r="S1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -858,9 +855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661158B2-352C-4F57-9B9E-C73E8105ACCC}">
   <dimension ref="A1:AA1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,82 +872,82 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="Z1" s="9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AA1" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
joined drops & stations sheets
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Rothfels\Documents\auto_qc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D986C827-F299-429F-BBA5-308F7A6B7D21}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2291F8B-5B3F-4063-97B5-E55F5259C521}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8175" xr2:uid="{DA3D1637-7497-4FA4-AFD8-B0930C0FCFB0}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>File</t>
   </si>
@@ -75,82 +75,10 @@
   </si>
   <si>
     <t>QA</t>
-  </si>
-  <si>
-    <t>SessionID</t>
-  </si>
-  <si>
-    <t>StationID</t>
-  </si>
-  <si>
-    <t>Station</t>
-  </si>
-  <si>
-    <t>StationUnit</t>
-  </si>
-  <si>
-    <t>StationDirection</t>
-  </si>
-  <si>
-    <t>LaneNumber</t>
-  </si>
-  <si>
-    <t>PavementType</t>
-  </si>
-  <si>
-    <t>Section No</t>
-  </si>
-  <si>
-    <t>SlabID</t>
-  </si>
-  <si>
-    <t>SlabPosition</t>
-  </si>
-  <si>
-    <t>SlabPositionCode</t>
-  </si>
-  <si>
-    <t>Asphalt</t>
-  </si>
-  <si>
-    <t>Surface</t>
-  </si>
-  <si>
-    <t>Air</t>
-  </si>
-  <si>
-    <t>Cracks</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>GPSStatus</t>
-  </si>
-  <si>
-    <t>Satellites</t>
-  </si>
-  <si>
-    <t>UTC</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>Height</t>
-  </si>
-  <si>
-    <t>Comment</t>
   </si>
   <si>
     <t xml:space="preserve">Date Collected
 </t>
-  </si>
-  <si>
-    <t>insufficient field tests</t>
   </si>
   <si>
     <t>Time Collected From</t>
@@ -169,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,14 +118,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,30 +134,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="22"/>
-        <bgColor indexed="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -269,45 +173,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -324,18 +195,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Sheet2" xfId="1" xr:uid="{E6FC81ED-C850-480A-890D-8E16747B0148}"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -734,7 +611,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="7" width="9.140625" style="7"/>
+    <col min="6" max="7" width="9.140625" style="5"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="10" max="10" width="10.140625" customWidth="1"/>
     <col min="19" max="19" width="10.42578125" customWidth="1"/>
@@ -742,84 +619,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="54" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" s="4" t="s">
+      <c r="S1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:BB1048576">
-    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Good"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Bad"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J1040000 S2:S1040000">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="2" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="2" stopIfTrue="1">
       <formula>LEN(TRIM(J2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -840,10 +717,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <conditionalFormatting sqref="A1:AZ1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -853,106 +730,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661158B2-352C-4F57-9B9E-C73E8105ACCC}">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="25" max="25" width="20.5703125" customWidth="1"/>
-    <col min="26" max="26" width="11.140625" style="8" customWidth="1"/>
+    <col min="26" max="26" width="11.140625" style="6" customWidth="1"/>
     <col min="27" max="27" width="11.85546875" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA1" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="Z2:AA104857">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <sheetData/>
+  <conditionalFormatting sqref="A1:BZ1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added check station < section length
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Rothfels\Documents\auto_qc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2291F8B-5B3F-4063-97B5-E55F5259C521}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CF2E0E-B6AF-4AE0-9AB5-582614C048C6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8175" xr2:uid="{DA3D1637-7497-4FA4-AFD8-B0930C0FCFB0}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>File</t>
   </si>
@@ -91,13 +91,16 @@
   </si>
   <si>
     <t>Decreasing Deflections</t>
+  </si>
+  <si>
+    <t>Station &lt; Section Length</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,12 +113,6 @@
       <sz val="9"/>
       <color theme="0"/>
       <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -202,12 +199,22 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFCEFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
@@ -235,9 +242,29 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFCEFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
@@ -255,6 +282,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -275,11 +322,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -287,10 +334,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9C0006"/>
+      <color rgb="FFFFCEFF"/>
       <color rgb="FF006100"/>
       <color rgb="FFC6EFCE"/>
       <color rgb="FFFFC7CE"/>
-      <color rgb="FF9C0006"/>
       <color rgb="FFFFFFFF"/>
     </mruColors>
   </colors>
@@ -602,11 +650,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{328796CE-C1EE-4EC0-BFDD-AD4395456B69}">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,11 +662,11 @@
     <col min="6" max="7" width="9.140625" style="5"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" customWidth="1"/>
+    <col min="19" max="20" width="10.42578125" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="54" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -677,27 +725,35 @@
         <v>20</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:BB1048576">
-    <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="A1:BC1048576">
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Good"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Bad"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J1040000 S2:S1040000">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="2" stopIfTrue="1">
+  <conditionalFormatting sqref="J2:J1040000 S2:T1040000">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(J2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:BZ1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"O"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -717,10 +773,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <conditionalFormatting sqref="A1:AZ1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" stopIfTrue="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -745,7 +801,7 @@
   </cols>
   <sheetData/>
   <conditionalFormatting sqref="A1:BZ1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
bug fixes after first run
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Rothfels\Documents\auto_qc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erothfels\Documents\qc_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CF2E0E-B6AF-4AE0-9AB5-582614C048C6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FF416E-1C14-403E-9738-2A27B9355034}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8175" xr2:uid="{DA3D1637-7497-4FA4-AFD8-B0930C0FCFB0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8175" activeTab="3" xr2:uid="{DA3D1637-7497-4FA4-AFD8-B0930C0FCFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
     <sheet name="test list" sheetId="4" r:id="rId2"/>
     <sheet name="Stations" sheetId="3" r:id="rId3"/>
+    <sheet name="Stations &amp; Drops" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -199,7 +200,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -247,86 +288,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFCEFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -652,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{328796CE-C1EE-4EC0-BFDD-AD4395456B69}">
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
     </sheetView>
@@ -736,23 +697,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:BC1048576">
-    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Good"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Bad"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J1040000 S2:T1040000">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(J2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:BZ1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
       <formula>"O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -773,10 +734,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <conditionalFormatting sqref="A1:AZ1048576">
-    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -801,7 +762,32 @@
   </cols>
   <sheetData/>
   <conditionalFormatting sqref="A1:BZ1048576">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4665DCB6-4311-4103-9460-925BCA76E4B7}">
+  <dimension ref="Z1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="25" max="25" width="20.5703125" customWidth="1"/>
+    <col min="26" max="26" width="11.140625" style="6" customWidth="1"/>
+    <col min="27" max="27" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <conditionalFormatting sqref="A1:BZ1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added temp check inputs to gui
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erothfels\Documents\qc_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FF416E-1C14-403E-9738-2A27B9355034}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16496F3-BC51-47C1-95FC-FDA2149C5018}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8175" activeTab="3" xr2:uid="{DA3D1637-7497-4FA4-AFD8-B0930C0FCFB0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8175" xr2:uid="{DA3D1637-7497-4FA4-AFD8-B0930C0FCFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Stations" sheetId="3" r:id="rId3"/>
     <sheet name="Stations &amp; Drops" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,16 +51,10 @@
     <t>Max Station</t>
   </si>
   <si>
-    <t>Surface Temperature</t>
-  </si>
-  <si>
     <t>Min Surface Temp</t>
   </si>
   <si>
     <t>Max Surface Temp</t>
-  </si>
-  <si>
-    <t>Air Temperature</t>
   </si>
   <si>
     <t>Min Air Temp</t>
@@ -95,6 +89,12 @@
   </si>
   <si>
     <t>Station &lt; Section Length</t>
+  </si>
+  <si>
+    <t>Surface Temp Check</t>
+  </si>
+  <si>
+    <t>Air Temp Check</t>
   </si>
 </sst>
 </file>
@@ -613,9 +613,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{328796CE-C1EE-4EC0-BFDD-AD4395456B69}">
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,13 +629,13 @@
   <sheetData>
     <row r="1" spans="1:22" ht="54" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -656,43 +656,43 @@
         <v>5</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="Q1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="V1" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -774,7 +774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4665DCB6-4311-4103-9460-925BCA76E4B7}">
   <dimension ref="Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
     </sheetView>

</xml_diff>

<commit_message>
added # of stations stat
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erothfels\Documents\qc_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16496F3-BC51-47C1-95FC-FDA2149C5018}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D4777C-7542-408B-98D7-578AC8B885AB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8175" xr2:uid="{DA3D1637-7497-4FA4-AFD8-B0930C0FCFB0}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>File</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>TO</t>
-  </si>
-  <si>
-    <t>Completed Tests</t>
   </si>
   <si>
     <t>Lane</t>
@@ -95,6 +92,12 @@
   </si>
   <si>
     <t>Air Temp Check</t>
+  </si>
+  <si>
+    <t>Number of Stations</t>
+  </si>
+  <si>
+    <t>Number of Drops</t>
   </si>
 </sst>
 </file>
@@ -611,31 +614,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{328796CE-C1EE-4EC0-BFDD-AD4395456B69}">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="7" width="9.140625" style="5"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="19" max="20" width="10.42578125" customWidth="1"/>
-    <col min="21" max="21" width="11.28515625" customWidth="1"/>
+    <col min="6" max="8" width="9.140625" style="5"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="20" max="21" width="10.42578125" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="54" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -649,54 +652,57 @@
       <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="R1" s="7" t="s">
+      <c r="U1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:BC1048576">
+  <conditionalFormatting sqref="A1:BD1048576">
     <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
@@ -707,12 +713,12 @@
       <formula>"Bad"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J1040000 S2:T1040000">
+  <conditionalFormatting sqref="K2:K1040000 T2:U1040000">
     <cfRule type="notContainsBlanks" dxfId="5" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(J2))&gt;0</formula>
+      <formula>LEN(TRIM(K2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:BZ1048576">
+  <conditionalFormatting sqref="A1:CA1048576">
     <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
       <formula>"O"</formula>
     </cfRule>

</xml_diff>